<commit_message>
ExcelData provider issue fixed.
</commit_message>
<xml_diff>
--- a/FrameWork/Testdata/TestData2.xlsx
+++ b/FrameWork/Testdata/TestData2.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Login" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>ranjan36</t>
+    <t>abcdefg</t>
+  </si>
+  <si>
+    <t>dfdsdsd</t>
   </si>
 </sst>
 </file>
@@ -350,81 +351,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1">
-        <v>9837308375</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>9837308375</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1">
-        <v>9837308375</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>9837308375</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>